<commit_message>
fix: mute patient on transfer (#279)
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/patient_transferred_outcome.xlsx
+++ b/itech-malawi/forms/app/patient_transferred_outcome.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
   <si>
     <t>type</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Patient Phone Number</t>
+  </si>
+  <si>
+    <t>transferred_out</t>
+  </si>
+  <si>
+    <t>Transferred Out</t>
   </si>
   <si>
     <t>n</t>
@@ -199,61 +205,115 @@
     <t>Patient Name: ${patient_name}</t>
   </si>
   <si>
+    <t>_contact_phone</t>
+  </si>
+  <si>
+    <t>Patient Phone Number: ${patient_phone}</t>
+  </si>
+  <si>
+    <t>_national_id</t>
+  </si>
+  <si>
+    <t>National ID: ${national_id}</t>
+  </si>
+  <si>
+    <t>_filing_number</t>
+  </si>
+  <si>
+    <t>Filing Number: ${filing_number}</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>${request_id}</t>
+  </si>
+  <si>
+    <t>date_requested</t>
+  </si>
+  <si>
+    <t>${request_date}</t>
+  </si>
+  <si>
+    <t>select_one yes_remindme_others</t>
+  </si>
+  <si>
+    <t>client_ok</t>
+  </si>
+  <si>
+    <t>Have you notified the back to care team?</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>additional_notes</t>
+  </si>
+  <si>
+    <t>Please explain</t>
+  </si>
+  <si>
+    <t>selected(../client_ok, ’others’)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>field-list summary</t>
+  </si>
+  <si>
+    <t>task_label</t>
+  </si>
+  <si>
+    <t>Task Label</t>
+  </si>
+  <si>
     <t>h1 blue</t>
   </si>
   <si>
-    <t>_contact_phone</t>
-  </si>
-  <si>
-    <t>Patient Phone Number: ${patient_phone}</t>
-  </si>
-  <si>
-    <t>_national_id</t>
-  </si>
-  <si>
-    <t>National ID: ${national_id}</t>
-  </si>
-  <si>
-    <t>_filing_number</t>
-  </si>
-  <si>
-    <t>Filing Number: ${filing_number}</t>
-  </si>
-  <si>
-    <t>request</t>
-  </si>
-  <si>
-    <t>${request_id}</t>
-  </si>
-  <si>
-    <t>date_requested</t>
-  </si>
-  <si>
-    <t>${request_date}</t>
-  </si>
-  <si>
-    <t>select_one yes_remindme_others</t>
-  </si>
-  <si>
-    <t>client_ok</t>
-  </si>
-  <si>
-    <t>Have you notified the back to care team?</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>additional_notes</t>
-  </si>
-  <si>
-    <t>Please explain</t>
-  </si>
-  <si>
-    <t>selected(../client_ok, ’others’)</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>warning</t>
+  </si>
+  <si>
+    <t>Be sure to submit to complete this action</t>
+  </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Form description: Complete form if patient transferred clinic. Please note that the patient will no longer receive study messages when you submit this form.</t>
+  </si>
+  <si>
+    <t>patient_details</t>
+  </si>
+  <si>
+    <t>Patient Details</t>
+  </si>
+  <si>
+    <t>h1 yellow</t>
+  </si>
+  <si>
+    <t>_findings</t>
+  </si>
+  <si>
+    <t>Findings</t>
+  </si>
+  <si>
+    <t>_outcome</t>
+  </si>
+  <si>
+    <t>Notified Back to Care?: ${client_ok}</t>
+  </si>
+  <si>
+    <t>_explanation</t>
+  </si>
+  <si>
+    <t>Notes: ${additional_notes}</t>
   </si>
   <si>
     <t>list_name</t>
@@ -391,7 +451,7 @@
       <name val="Proxima Nova"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +503,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -558,16 +630,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="18"/>
+        <color indexed="20"/>
       </left>
       <right style="thin">
-        <color indexed="18"/>
+        <color indexed="20"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="20"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,7 +651,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="20"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -592,7 +664,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -707,6 +779,12 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
@@ -737,6 +815,36 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -764,10 +872,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -804,6 +912,8 @@
       <rgbColor rgb="fffbd4b4"/>
       <rgbColor rgb="ff95b3d7"/>
       <rgbColor rgb="ffb8cce4"/>
+      <rgbColor rgb="ff9bbb59"/>
+      <rgbColor rgb="ffcdddac"/>
       <rgbColor rgb="ff2e75b6"/>
       <rgbColor rgb="ffd0cece"/>
     </indexedColors>
@@ -1867,11 +1977,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.3333" defaultRowHeight="16.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="34.8516" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.1719" style="1" customWidth="1"/>
@@ -2541,7 +2651,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" t="s" s="33">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s" s="34">
         <v>54</v>
@@ -2551,14 +2661,20 @@
       </c>
       <c r="D19" s="36"/>
       <c r="E19" t="s" s="34">
-        <v>16</v>
-      </c>
-      <c r="F19" s="36"/>
+        <v>20</v>
+      </c>
+      <c r="F19" t="s" s="34">
+        <v>34</v>
+      </c>
       <c r="G19" s="36"/>
       <c r="H19" s="36"/>
       <c r="I19" s="37"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="37"/>
+      <c r="J19" t="b" s="38">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b" s="39">
+        <v>1</v>
+      </c>
       <c r="L19" s="37"/>
       <c r="M19" s="31"/>
       <c r="N19" s="32"/>
@@ -2575,27 +2691,27 @@
       <c r="Y19" s="32"/>
       <c r="Z19" s="32"/>
     </row>
-    <row r="20" ht="228.75" customHeight="1">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" t="s" s="33">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s" s="34">
         <v>56</v>
       </c>
-      <c r="B20" t="s" s="34">
+      <c r="C20" t="s" s="35">
         <v>57</v>
       </c>
-      <c r="C20" t="s" s="38">
-        <v>58</v>
-      </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="40"/>
-      <c r="L20" t="s" s="41">
-        <v>20</v>
-      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" t="s" s="34">
+        <v>16</v>
+      </c>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
       <c r="M20" s="31"/>
       <c r="N20" s="32"/>
       <c r="O20" s="32"/>
@@ -2611,27 +2727,27 @@
       <c r="Y20" s="32"/>
       <c r="Z20" s="32"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" ht="228.75" customHeight="1">
       <c r="A21" t="s" s="33">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s" s="34">
         <v>59</v>
       </c>
-      <c r="C21" t="s" s="42">
+      <c r="C21" t="s" s="40">
         <v>60</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" t="s" s="42">
-        <v>61</v>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="42"/>
+      <c r="L21" t="s" s="43">
+        <v>20</v>
+      </c>
       <c r="M21" s="31"/>
       <c r="N21" s="32"/>
       <c r="O21" s="32"/>
@@ -2649,23 +2765,23 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" t="s" s="33">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s" s="34">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s" s="44">
         <v>62</v>
       </c>
-      <c r="C22" t="s" s="42">
-        <v>63</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="31"/>
       <c r="N22" s="32"/>
       <c r="O22" s="32"/>
@@ -2683,23 +2799,23 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" t="s" s="33">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s" s="34">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s" s="44">
         <v>64</v>
       </c>
-      <c r="C23" t="s" s="42">
-        <v>65</v>
-      </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
       <c r="M23" s="31"/>
       <c r="N23" s="32"/>
       <c r="O23" s="32"/>
@@ -2717,23 +2833,23 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" t="s" s="33">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s" s="34">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s" s="44">
         <v>66</v>
       </c>
-      <c r="C24" t="s" s="42">
-        <v>67</v>
-      </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
       <c r="M24" s="31"/>
       <c r="N24" s="32"/>
       <c r="O24" s="32"/>
@@ -2751,25 +2867,23 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" t="s" s="33">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s" s="34">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s" s="44">
         <v>68</v>
       </c>
-      <c r="C25" t="s" s="42">
-        <v>55</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" t="s" s="42">
-        <v>20</v>
-      </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
       <c r="M25" s="31"/>
       <c r="N25" s="32"/>
       <c r="O25" s="32"/>
@@ -2787,25 +2901,25 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" t="s" s="33">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s" s="34">
-        <v>31</v>
-      </c>
-      <c r="C26" t="s" s="42">
-        <v>55</v>
-      </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="39"/>
-      <c r="K26" t="s" s="41">
         <v>69</v>
       </c>
-      <c r="L26" s="40"/>
+      <c r="C26" t="s" s="44">
+        <v>57</v>
+      </c>
+      <c r="D26" s="41"/>
+      <c r="E26" t="s" s="44">
+        <v>20</v>
+      </c>
+      <c r="F26" s="44"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
       <c r="M26" s="31"/>
       <c r="N26" s="32"/>
       <c r="O26" s="32"/>
@@ -2826,22 +2940,22 @@
         <v>44</v>
       </c>
       <c r="B27" t="s" s="34">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s" s="44">
+        <v>57</v>
+      </c>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="41"/>
+      <c r="K27" t="s" s="43">
         <v>70</v>
       </c>
-      <c r="C27" t="s" s="42">
-        <v>55</v>
-      </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="39"/>
-      <c r="K27" t="s" s="41">
-        <v>71</v>
-      </c>
-      <c r="L27" s="40"/>
+      <c r="L27" s="42"/>
       <c r="M27" s="31"/>
       <c r="N27" s="32"/>
       <c r="O27" s="32"/>
@@ -2859,19 +2973,25 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" t="s" s="33">
-        <v>43</v>
-      </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
+        <v>44</v>
+      </c>
+      <c r="B28" t="s" s="34">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s" s="44">
+        <v>57</v>
+      </c>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="41"/>
+      <c r="K28" t="s" s="43">
+        <v>72</v>
+      </c>
+      <c r="L28" s="42"/>
       <c r="M28" s="31"/>
       <c r="N28" s="32"/>
       <c r="O28" s="32"/>
@@ -2889,25 +3009,19 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" t="s" s="33">
-        <v>72</v>
-      </c>
-      <c r="B29" t="s" s="34">
-        <v>73</v>
-      </c>
-      <c r="C29" t="s" s="42">
-        <v>74</v>
-      </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" t="s" s="42">
-        <v>34</v>
-      </c>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
+        <v>43</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
       <c r="M29" s="31"/>
       <c r="N29" s="32"/>
       <c r="O29" s="32"/>
@@ -2925,27 +3039,25 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" t="s" s="33">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s" s="34">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s" s="44">
         <v>75</v>
       </c>
-      <c r="B30" t="s" s="34">
-        <v>76</v>
-      </c>
-      <c r="C30" t="s" s="43">
-        <v>77</v>
-      </c>
-      <c r="D30" t="s" s="42">
-        <v>78</v>
-      </c>
-      <c r="E30" s="39"/>
-      <c r="F30" t="s" s="42">
-        <v>79</v>
-      </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" t="s" s="44">
+        <v>34</v>
+      </c>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
       <c r="M30" s="31"/>
       <c r="N30" s="32"/>
       <c r="O30" s="32"/>
@@ -2962,21 +3074,29 @@
       <c r="Z30" s="32"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" t="s" s="44">
-        <v>43</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="47"/>
+      <c r="A31" t="s" s="33">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s" s="34">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s" s="45">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s" s="44">
+        <v>79</v>
+      </c>
+      <c r="E31" s="41"/>
+      <c r="F31" t="s" s="44">
+        <v>80</v>
+      </c>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="31"/>
       <c r="N31" s="32"/>
       <c r="O31" s="32"/>
       <c r="P31" s="32"/>
@@ -2990,6 +3110,484 @@
       <c r="X31" s="32"/>
       <c r="Y31" s="32"/>
       <c r="Z31" s="32"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" t="s" s="46">
+        <v>43</v>
+      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" t="s" s="50">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s" s="51">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s" s="52">
+        <v>57</v>
+      </c>
+      <c r="D33" s="53"/>
+      <c r="E33" t="s" s="54">
+        <v>82</v>
+      </c>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="32"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="32"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" t="s" s="50">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s" s="51">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s" s="52">
+        <v>84</v>
+      </c>
+      <c r="D34" s="53"/>
+      <c r="E34" t="s" s="54">
+        <v>85</v>
+      </c>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="32"/>
+      <c r="R34" s="32"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="32"/>
+      <c r="U34" s="32"/>
+      <c r="V34" s="32"/>
+      <c r="W34" s="32"/>
+      <c r="X34" s="32"/>
+      <c r="Y34" s="32"/>
+      <c r="Z34" s="32"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" t="s" s="50">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s" s="51">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s" s="52">
+        <v>87</v>
+      </c>
+      <c r="D35" s="53"/>
+      <c r="E35" t="s" s="54">
+        <v>88</v>
+      </c>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="32"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="32"/>
+      <c r="W35" s="32"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="32"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" t="s" s="50">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s" s="51">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s" s="52">
+        <v>90</v>
+      </c>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="32"/>
+      <c r="R36" s="32"/>
+      <c r="S36" s="32"/>
+      <c r="T36" s="32"/>
+      <c r="U36" s="32"/>
+      <c r="V36" s="32"/>
+      <c r="W36" s="32"/>
+      <c r="X36" s="32"/>
+      <c r="Y36" s="32"/>
+      <c r="Z36" s="32"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" t="s" s="50">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s" s="51">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s" s="52">
+        <v>92</v>
+      </c>
+      <c r="D37" s="53"/>
+      <c r="E37" t="s" s="54">
+        <v>93</v>
+      </c>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B38" t="s" s="57">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s" s="58">
+        <v>62</v>
+      </c>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="32"/>
+      <c r="S38" s="32"/>
+      <c r="T38" s="32"/>
+      <c r="U38" s="32"/>
+      <c r="V38" s="32"/>
+      <c r="W38" s="32"/>
+      <c r="X38" s="32"/>
+      <c r="Y38" s="32"/>
+      <c r="Z38" s="32"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B39" t="s" s="57">
+        <v>63</v>
+      </c>
+      <c r="C39" t="s" s="58">
+        <v>64</v>
+      </c>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="32"/>
+      <c r="R39" s="32"/>
+      <c r="S39" s="32"/>
+      <c r="T39" s="32"/>
+      <c r="U39" s="32"/>
+      <c r="V39" s="32"/>
+      <c r="W39" s="32"/>
+      <c r="X39" s="32"/>
+      <c r="Y39" s="32"/>
+      <c r="Z39" s="32"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s" s="57">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s" s="58">
+        <v>66</v>
+      </c>
+      <c r="D40" s="53"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="32"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="32"/>
+      <c r="W40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="32"/>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B41" t="s" s="57">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s" s="58">
+        <v>68</v>
+      </c>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="32"/>
+      <c r="Q41" s="32"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="32"/>
+      <c r="T41" s="32"/>
+      <c r="U41" s="32"/>
+      <c r="V41" s="32"/>
+      <c r="W41" s="32"/>
+      <c r="X41" s="32"/>
+      <c r="Y41" s="32"/>
+      <c r="Z41" s="32"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s" s="57">
+        <v>94</v>
+      </c>
+      <c r="C42" t="s" s="58">
+        <v>95</v>
+      </c>
+      <c r="D42" s="53"/>
+      <c r="E42" t="s" s="54">
+        <v>85</v>
+      </c>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32"/>
+      <c r="Q42" s="32"/>
+      <c r="R42" s="32"/>
+      <c r="S42" s="32"/>
+      <c r="T42" s="32"/>
+      <c r="U42" s="32"/>
+      <c r="V42" s="32"/>
+      <c r="W42" s="32"/>
+      <c r="X42" s="32"/>
+      <c r="Y42" s="32"/>
+      <c r="Z42" s="32"/>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B43" t="s" s="57">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s" s="58">
+        <v>97</v>
+      </c>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32"/>
+      <c r="Q43" s="32"/>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="32"/>
+      <c r="V43" s="32"/>
+      <c r="W43" s="32"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="32"/>
+      <c r="Z43" s="32"/>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" t="s" s="56">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s" s="57">
+        <v>98</v>
+      </c>
+      <c r="C44" t="s" s="58">
+        <v>99</v>
+      </c>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="32"/>
+      <c r="Q44" s="32"/>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="32"/>
+      <c r="V44" s="32"/>
+      <c r="W44" s="32"/>
+      <c r="X44" s="32"/>
+      <c r="Y44" s="32"/>
+      <c r="Z44" s="32"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" t="s" s="50">
+        <v>43</v>
+      </c>
+      <c r="B45" s="59"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="32"/>
+      <c r="Q45" s="32"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="32"/>
+      <c r="V45" s="32"/>
+      <c r="W45" s="32"/>
+      <c r="X45" s="32"/>
+      <c r="Y45" s="32"/>
+      <c r="Z45" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>
@@ -3008,68 +3606,68 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="48" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="48" customWidth="1"/>
-    <col min="3" max="3" width="17.8516" style="48" customWidth="1"/>
-    <col min="4" max="5" width="11.5" style="48" customWidth="1"/>
-    <col min="6" max="16384" width="11.3516" style="48" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="60" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="17.8516" style="60" customWidth="1"/>
+    <col min="4" max="5" width="11.5" style="60" customWidth="1"/>
+    <col min="6" max="16384" width="11.3516" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" t="s" s="49">
-        <v>80</v>
-      </c>
-      <c r="B1" t="s" s="49">
+      <c r="A1" t="s" s="61">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s" s="61">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="49">
+      <c r="C1" t="s" s="61">
         <v>2</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" t="s" s="51">
-        <v>81</v>
-      </c>
-      <c r="B3" t="s" s="51">
+      <c r="A3" t="s" s="63">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s" s="63">
         <v>34</v>
       </c>
-      <c r="C3" t="s" s="51">
-        <v>82</v>
+      <c r="C3" t="s" s="63">
+        <v>102</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" t="s" s="51">
-        <v>81</v>
-      </c>
-      <c r="B4" t="s" s="51">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s" s="51">
-        <v>84</v>
+      <c r="A4" t="s" s="63">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s" s="63">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s" s="63">
+        <v>104</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" t="s" s="51">
-        <v>81</v>
-      </c>
-      <c r="B5" t="s" s="52">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s" s="52">
-        <v>86</v>
+      <c r="A5" t="s" s="63">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s" s="64">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s" s="64">
+        <v>106</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -3098,16 +3696,16 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="50"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>
@@ -3126,104 +3724,104 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.8516" style="56" customWidth="1"/>
-    <col min="2" max="2" width="43.6719" style="56" customWidth="1"/>
-    <col min="3" max="3" width="32.8516" style="56" customWidth="1"/>
-    <col min="4" max="4" width="20.8516" style="56" customWidth="1"/>
-    <col min="5" max="15" width="11.5" style="56" customWidth="1"/>
-    <col min="16" max="26" width="8.85156" style="56" customWidth="1"/>
-    <col min="27" max="16384" width="11.3516" style="56" customWidth="1"/>
+    <col min="1" max="1" width="31.8516" style="68" customWidth="1"/>
+    <col min="2" max="2" width="43.6719" style="68" customWidth="1"/>
+    <col min="3" max="3" width="32.8516" style="68" customWidth="1"/>
+    <col min="4" max="4" width="20.8516" style="68" customWidth="1"/>
+    <col min="5" max="15" width="11.5" style="68" customWidth="1"/>
+    <col min="16" max="26" width="8.85156" style="68" customWidth="1"/>
+    <col min="27" max="16384" width="11.3516" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
-      <c r="A1" t="s" s="57">
-        <v>87</v>
-      </c>
-      <c r="B1" t="s" s="57">
-        <v>88</v>
-      </c>
-      <c r="C1" t="s" s="57">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s" s="57">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s" s="57">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s" s="57">
-        <v>92</v>
-      </c>
-      <c r="G1" t="s" s="57">
+      <c r="A1" t="s" s="69">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s" s="69">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s" s="69">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s" s="69">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s" s="69">
+        <v>111</v>
+      </c>
+      <c r="F1" t="s" s="69">
+        <v>112</v>
+      </c>
+      <c r="G1" t="s" s="69">
         <v>1</v>
       </c>
-      <c r="H1" t="s" s="57">
-        <v>93</v>
-      </c>
-      <c r="I1" t="s" s="57">
-        <v>94</v>
-      </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
+      <c r="H1" t="s" s="69">
+        <v>113</v>
+      </c>
+      <c r="I1" t="s" s="69">
+        <v>114</v>
+      </c>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" t="s" s="59">
-        <v>95</v>
-      </c>
-      <c r="B2" t="s" s="60">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s" s="60">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s" s="60">
-        <v>98</v>
-      </c>
-      <c r="E2" t="s" s="60">
-        <v>99</v>
-      </c>
-      <c r="F2" s="61"/>
-      <c r="G2" t="s" s="60">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s" s="60">
-        <v>100</v>
-      </c>
-      <c r="I2" t="s" s="60">
-        <v>101</v>
-      </c>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
+      <c r="A2" t="s" s="71">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s" s="72">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s" s="72">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s" s="72">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s" s="72">
+        <v>119</v>
+      </c>
+      <c r="F2" s="73"/>
+      <c r="G2" t="s" s="72">
+        <v>120</v>
+      </c>
+      <c r="H2" t="s" s="72">
+        <v>120</v>
+      </c>
+      <c r="I2" t="s" s="72">
+        <v>121</v>
+      </c>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="Z2" s="73"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" s="4"/>

</xml_diff>